<commit_message>
P3_Analysis : analyse temporelle des proportions des pnns1, de nutrigrade, des teneurs pour 100g et du nutriscore + rédaction + boxplots et préparation ANOVA
</commit_message>
<xml_diff>
--- a/Nettoyage.xlsx
+++ b/Nettoyage.xlsx
@@ -247,11 +247,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="136581632"/>
-        <c:axId val="136581056"/>
+        <c:axId val="35206208"/>
+        <c:axId val="35206784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="136581632"/>
+        <c:axId val="35206208"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -298,7 +298,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="136581056"/>
+        <c:crossAx val="35206784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -306,7 +306,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="136581056"/>
+        <c:axId val="35206784"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -336,7 +336,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136581632"/>
+        <c:crossAx val="35206208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -474,11 +474,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="135460352"/>
-        <c:axId val="610887936"/>
+        <c:axId val="133355520"/>
+        <c:axId val="35208512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="135460352"/>
+        <c:axId val="133355520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -488,7 +488,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="610887936"/>
+        <c:crossAx val="35208512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -496,7 +496,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="610887936"/>
+        <c:axId val="35208512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -530,7 +530,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135460352"/>
+        <c:crossAx val="133355520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -673,11 +673,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="142325952"/>
-        <c:axId val="142325376"/>
+        <c:axId val="135046272"/>
+        <c:axId val="135046848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="142325952"/>
+        <c:axId val="135046272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -686,12 +686,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142325376"/>
+        <c:crossAx val="135046848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="142325376"/>
+        <c:axId val="135046848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -701,7 +701,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142325952"/>
+        <c:crossAx val="135046272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -796,15 +796,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2207559</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>100854</xdr:rowOff>
+      <xdr:colOff>2554942</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>123265</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>369794</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:colOff>717177</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1272,7 +1272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A7:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
@@ -1325,7 +1325,7 @@
         <v>251045914</v>
       </c>
       <c r="H10">
-        <f>100-I10</f>
+        <f t="shared" ref="H10:H15" si="0">100-I10</f>
         <v>21.5</v>
       </c>
       <c r="I10">
@@ -1346,11 +1346,11 @@
         <v>44</v>
       </c>
       <c r="G11">
-        <f t="shared" ref="G11:G15" si="0">C11*E11</f>
+        <f t="shared" ref="G11:G15" si="1">C11*E11</f>
         <v>61027736</v>
       </c>
       <c r="H11">
-        <f>100-I11</f>
+        <f t="shared" si="0"/>
         <v>50.6</v>
       </c>
       <c r="I11">
@@ -1371,11 +1371,11 @@
         <v>47</v>
       </c>
       <c r="G12">
+        <f t="shared" si="1"/>
+        <v>65188718</v>
+      </c>
+      <c r="H12">
         <f t="shared" si="0"/>
-        <v>65188718</v>
-      </c>
-      <c r="H12">
-        <f>100-I12</f>
         <v>63</v>
       </c>
       <c r="I12">
@@ -1396,11 +1396,11 @@
         <v>47</v>
       </c>
       <c r="G13">
+        <f t="shared" si="1"/>
+        <v>65162069</v>
+      </c>
+      <c r="H13">
         <f t="shared" si="0"/>
-        <v>65162069</v>
-      </c>
-      <c r="H13">
-        <f>100-I13</f>
         <v>63</v>
       </c>
       <c r="I13">
@@ -1421,11 +1421,11 @@
         <v>46</v>
       </c>
       <c r="G14">
+        <f t="shared" si="1"/>
+        <v>25943540</v>
+      </c>
+      <c r="H14">
         <f t="shared" si="0"/>
-        <v>25943540</v>
-      </c>
-      <c r="H14">
-        <f>100-I14</f>
         <v>79.7</v>
       </c>
       <c r="I14">
@@ -1446,11 +1446,11 @@
         <v>46</v>
       </c>
       <c r="G15">
+        <f t="shared" si="1"/>
+        <v>25943540</v>
+      </c>
+      <c r="H15">
         <f t="shared" si="0"/>
-        <v>25943540</v>
-      </c>
-      <c r="H15">
-        <f>100-I15</f>
         <v>100</v>
       </c>
       <c r="I15">

</xml_diff>